<commit_message>
Testcase for 1.1.4 is uploaded
</commit_message>
<xml_diff>
--- a/Master-functional-testcases/Pre-registration/TC_PreRegistration.xlsx
+++ b/Master-functional-testcases/Pre-registration/TC_PreRegistration.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jane.rose\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niyati.Swami\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-reg" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="1.2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pre-reg'!$A$1:$G$133</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pre-reg'!$A$1:$G$154</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="567">
   <si>
     <t xml:space="preserve">TestCase_No </t>
   </si>
@@ -1639,11 +1639,157 @@
   <si>
     <t>Under UI the if user doesnot fill the data under POI , POA user should not be able to move ahead if the fields are mandatory</t>
   </si>
+  <si>
+    <t xml:space="preserve">To add the Document Number textbox under UI Schema with Document Upload </t>
+  </si>
+  <si>
+    <t>The User should be able to add the document Number textbox type with alignment similar to Document Upload</t>
+  </si>
+  <si>
+    <t>To add the Document Number textbox under UI Schema with Document Upload as Mandatory Field</t>
+  </si>
+  <si>
+    <t>The User should be able to add the document Number textbox type with alignment similar to Document Upload and UI should not allow to move ahead incase the field as the field is mandatory</t>
+  </si>
+  <si>
+    <t>To add the Document Number textbox under UI Schema with Document Upload as Non-Mandatory Field</t>
+  </si>
+  <si>
+    <t>The User should leave the document Number textbox type with alignment similar to Document Upload and UI should be allow to move ahead incase the field as the field is non- mandatory</t>
+  </si>
+  <si>
+    <t>To verify that Document number is copied when the document uploaded is copied for other applicant</t>
+  </si>
+  <si>
+    <t>The Document Number should be populated with the doc copied for applicant for POA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that Document  Number to fetched in regclient when PRID is synced </t>
+  </si>
+  <si>
+    <t>The Document Number should be populated with the doc uploaded in regclient application</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_23</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_24</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_25</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_26</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_27</t>
+  </si>
+  <si>
+    <t>Reviwed</t>
+  </si>
+  <si>
+    <t>To verify that UI schema should have multiple address support</t>
+  </si>
+  <si>
+    <t>The user should able to add multiple address in UI schema and that should be populated in pre registration demographic UI page</t>
+  </si>
+  <si>
+    <t>To verify that UI schema should have multiple hierarchy support</t>
+  </si>
+  <si>
+    <t>The user should be allowed to add the hierarchy as per the wish as 
+for Place of Birth : Country&gt;&gt; Province&gt;&gt; City
+For temp address&gt;&gt; Country&gt;&gt; Province&gt;&gt; City&gt;&gt; Barangay</t>
+  </si>
+  <si>
+    <t>To verify that user should be able to add same address with in the country in permanent and present address</t>
+  </si>
+  <si>
+    <t>The user should able to add same address with in the country in a permanent and present address</t>
+  </si>
+  <si>
+    <t>To verify that user should be able to add different address with in the country in permanent and present address</t>
+  </si>
+  <si>
+    <t>To verify that user should be able to add different address choosing different country  in permanent and present address</t>
+  </si>
+  <si>
+    <t>The user should be allowed to add the address for different country</t>
+  </si>
+  <si>
+    <t>To verify the behavior by adding POB</t>
+  </si>
+  <si>
+    <t>The should be able to get the details in dropdown and should be able to select the same</t>
+  </si>
+  <si>
+    <t>To verify the behavior by adding temporary address with same hirearchy as present address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify POB and Address added should appear in regclient </t>
+  </si>
+  <si>
+    <t>The data filled under pre-reg should appear successfully in regclient.</t>
+  </si>
+  <si>
+    <t>To verify the presence of address in Preview page and acknowledgement page</t>
+  </si>
+  <si>
+    <t>The details added under demographic page should be there in Ack and Preview page.</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_11</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_12</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_13</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_14</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_15</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_16</t>
+  </si>
+  <si>
+    <t>Pre Registration_Demographic_17</t>
+  </si>
+  <si>
+    <t>To verify the encryption of data to get when data sync api is executed</t>
+  </si>
+  <si>
+    <t>The response should be received in encrypted format.</t>
+  </si>
+  <si>
+    <t>All the data filled under the pre-rge should be properly render under Regclient</t>
+  </si>
+  <si>
+    <t>Pre Registration_API_01</t>
+  </si>
+  <si>
+    <t>Pre Registration_API_02</t>
+  </si>
+  <si>
+    <t>Pre Registration_API_03</t>
+  </si>
+  <si>
+    <t>To verifythe data to be populated after the data is reterived using PRID in regclient</t>
+  </si>
+  <si>
+    <t>To verify that API call should not be made directly to Admin</t>
+  </si>
+  <si>
+    <t>The API call should be made through pre-reg not direct to masterData</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6">
     <font>
       <sz val="11"/>
@@ -1704,7 +1850,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1740,11 +1886,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1795,6 +1952,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2076,10 +2243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G552"/>
+  <dimension ref="A1:H552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134:G138"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H159" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2093,7 +2260,7 @@
     <col min="7" max="7" width="12.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2115,8 +2282,11 @@
       <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="89.25">
+      <c r="H1" s="20" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="89.25">
       <c r="A2" s="7" t="s">
         <v>271</v>
       </c>
@@ -2139,7 +2309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="63.75">
+    <row r="3" spans="1:8" ht="63.75">
       <c r="A3" s="7" t="s">
         <v>272</v>
       </c>
@@ -2162,7 +2332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="38.25">
+    <row r="4" spans="1:8" ht="38.25">
       <c r="A4" s="7" t="s">
         <v>273</v>
       </c>
@@ -2185,7 +2355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="76.5">
+    <row r="5" spans="1:8" ht="76.5">
       <c r="A5" s="7" t="s">
         <v>274</v>
       </c>
@@ -2208,7 +2378,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="25.5">
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="7" t="s">
         <v>275</v>
       </c>
@@ -2231,7 +2401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="38.25">
+    <row r="7" spans="1:8" ht="38.25">
       <c r="A7" s="7" t="s">
         <v>276</v>
       </c>
@@ -2254,7 +2424,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="25.5">
+    <row r="8" spans="1:8" ht="25.5">
       <c r="A8" s="7" t="s">
         <v>277</v>
       </c>
@@ -2277,7 +2447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="25.5">
+    <row r="9" spans="1:8" ht="25.5">
       <c r="A9" s="7" t="s">
         <v>278</v>
       </c>
@@ -2300,7 +2470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="38.25">
+    <row r="10" spans="1:8" ht="38.25">
       <c r="A10" s="7" t="s">
         <v>279</v>
       </c>
@@ -2321,7 +2491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="38.25">
+    <row r="11" spans="1:8" ht="38.25">
       <c r="A11" s="7" t="s">
         <v>280</v>
       </c>
@@ -2342,7 +2512,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="63.75">
+    <row r="12" spans="1:8" ht="63.75">
       <c r="A12" s="7" t="s">
         <v>303</v>
       </c>
@@ -2365,7 +2535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
         <v>304</v>
       </c>
@@ -2388,7 +2558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="51">
+    <row r="14" spans="1:8" ht="51">
       <c r="A14" s="7" t="s">
         <v>305</v>
       </c>
@@ -2411,7 +2581,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="51">
+    <row r="15" spans="1:8" ht="51">
       <c r="A15" s="7" t="s">
         <v>306</v>
       </c>
@@ -2434,7 +2604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="63.75">
+    <row r="16" spans="1:8" ht="63.75">
       <c r="A16" s="7" t="s">
         <v>307</v>
       </c>
@@ -2457,7 +2627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="51">
+    <row r="17" spans="1:8" ht="51">
       <c r="A17" s="7" t="s">
         <v>308</v>
       </c>
@@ -2480,7 +2650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="25.5">
+    <row r="18" spans="1:8" ht="25.5">
       <c r="A18" s="7" t="s">
         <v>309</v>
       </c>
@@ -2503,7 +2673,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="38.25">
+    <row r="19" spans="1:8" ht="38.25">
       <c r="A19" s="7" t="s">
         <v>310</v>
       </c>
@@ -2526,7 +2696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="63.75">
+    <row r="20" spans="1:8" ht="63.75">
       <c r="A20" s="7" t="s">
         <v>311</v>
       </c>
@@ -2548,8 +2718,9 @@
       <c r="G20" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="38.25">
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" ht="38.25">
       <c r="A21" s="7" t="s">
         <v>312</v>
       </c>
@@ -2571,8 +2742,9 @@
       <c r="G21" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" ht="25.5">
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" ht="25.5">
       <c r="A22" s="7" t="s">
         <v>313</v>
       </c>
@@ -2594,8 +2766,9 @@
       <c r="G22" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" ht="25.5">
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="25.5">
       <c r="A23" s="7" t="s">
         <v>314</v>
       </c>
@@ -2617,8 +2790,9 @@
       <c r="G23" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="25.5">
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" ht="25.5">
       <c r="A24" s="7" t="s">
         <v>315</v>
       </c>
@@ -2640,8 +2814,9 @@
       <c r="G24" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" ht="25.5">
+      <c r="H24" s="10"/>
+    </row>
+    <row r="25" spans="1:8" ht="25.5">
       <c r="A25" s="7" t="s">
         <v>316</v>
       </c>
@@ -2663,8 +2838,9 @@
       <c r="G25" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" ht="25.5">
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26" spans="1:8" ht="25.5">
       <c r="A26" s="7" t="s">
         <v>317</v>
       </c>
@@ -2686,8 +2862,9 @@
       <c r="G26" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="38.25">
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" ht="38.25">
       <c r="A27" s="7" t="s">
         <v>318</v>
       </c>
@@ -2709,8 +2886,9 @@
       <c r="G27" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" ht="25.5">
+      <c r="H27" s="10"/>
+    </row>
+    <row r="28" spans="1:8" ht="25.5">
       <c r="A28" s="7" t="s">
         <v>319</v>
       </c>
@@ -2732,8 +2910,9 @@
       <c r="G28" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" ht="38.25">
+      <c r="H28" s="10"/>
+    </row>
+    <row r="29" spans="1:8" ht="38.25">
       <c r="A29" s="7" t="s">
         <v>320</v>
       </c>
@@ -2755,8 +2934,9 @@
       <c r="G29" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" ht="38.25">
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" ht="38.25">
       <c r="A30" s="7" t="s">
         <v>321</v>
       </c>
@@ -2778,8 +2958,9 @@
       <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" ht="38.25">
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" ht="38.25">
       <c r="A31" s="7" t="s">
         <v>322</v>
       </c>
@@ -2801,8 +2982,9 @@
       <c r="G31" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="38.25">
+      <c r="H31" s="10"/>
+    </row>
+    <row r="32" spans="1:8" ht="38.25">
       <c r="A32" s="7" t="s">
         <v>323</v>
       </c>
@@ -2824,8 +3006,9 @@
       <c r="G32" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="25.5">
+      <c r="H32" s="10"/>
+    </row>
+    <row r="33" spans="1:8" ht="25.5">
       <c r="A33" s="7" t="s">
         <v>324</v>
       </c>
@@ -2847,8 +3030,9 @@
       <c r="G33" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="38.25">
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:8" ht="38.25">
       <c r="A34" s="7" t="s">
         <v>325</v>
       </c>
@@ -2870,8 +3054,9 @@
       <c r="G34" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="51">
+      <c r="H34" s="10"/>
+    </row>
+    <row r="35" spans="1:8" ht="51">
       <c r="A35" s="7" t="s">
         <v>326</v>
       </c>
@@ -2893,8 +3078,9 @@
       <c r="G35" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="10"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="7" t="s">
         <v>327</v>
       </c>
@@ -2916,8 +3102,9 @@
       <c r="G36" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="7" t="s">
         <v>328</v>
       </c>
@@ -2939,8 +3126,9 @@
       <c r="G37" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="38.25">
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" ht="38.25">
       <c r="A38" s="7" t="s">
         <v>329</v>
       </c>
@@ -2962,8 +3150,9 @@
       <c r="G38" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="25.5">
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:8" ht="25.5">
       <c r="A39" s="7" t="s">
         <v>330</v>
       </c>
@@ -2985,8 +3174,9 @@
       <c r="G39" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" ht="25.5">
+      <c r="H39" s="10"/>
+    </row>
+    <row r="40" spans="1:8" ht="25.5">
       <c r="A40" s="7" t="s">
         <v>331</v>
       </c>
@@ -3008,8 +3198,9 @@
       <c r="G40" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" ht="51">
+      <c r="H40" s="10"/>
+    </row>
+    <row r="41" spans="1:8" ht="51">
       <c r="A41" s="7" t="s">
         <v>332</v>
       </c>
@@ -3031,8 +3222,9 @@
       <c r="G41" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" ht="51">
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" ht="51">
       <c r="A42" s="7" t="s">
         <v>269</v>
       </c>
@@ -3055,7 +3247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="51">
+    <row r="43" spans="1:8" ht="51">
       <c r="A43" s="7" t="s">
         <v>270</v>
       </c>
@@ -3078,7 +3270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="63.75">
+    <row r="44" spans="1:8" ht="63.75">
       <c r="A44" s="7" t="s">
         <v>281</v>
       </c>
@@ -3101,7 +3293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="102">
+    <row r="45" spans="1:8" ht="102">
       <c r="A45" s="7" t="s">
         <v>282</v>
       </c>
@@ -3124,7 +3316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="63.75">
+    <row r="46" spans="1:8" ht="63.75">
       <c r="A46" s="7" t="s">
         <v>283</v>
       </c>
@@ -3147,7 +3339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="51">
+    <row r="47" spans="1:8" ht="51">
       <c r="A47" s="7" t="s">
         <v>284</v>
       </c>
@@ -3170,7 +3362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="25.5">
+    <row r="48" spans="1:8" ht="25.5">
       <c r="A48" s="7" t="s">
         <v>285</v>
       </c>
@@ -5031,7 +5223,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="25.5">
+    <row r="129" spans="1:8" ht="25.5">
       <c r="A129" s="7" t="s">
         <v>391</v>
       </c>
@@ -5054,7 +5246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="25.5">
+    <row r="130" spans="1:8" ht="25.5">
       <c r="A130" s="7" t="s">
         <v>392</v>
       </c>
@@ -5077,7 +5269,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="25.5">
+    <row r="131" spans="1:8" ht="25.5">
       <c r="A131" s="7" t="s">
         <v>393</v>
       </c>
@@ -5100,7 +5292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="25.5">
+    <row r="132" spans="1:8" ht="25.5">
       <c r="A132" s="7" t="s">
         <v>394</v>
       </c>
@@ -5123,7 +5315,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="51">
+    <row r="133" spans="1:8" ht="51">
       <c r="A133" s="7" t="s">
         <v>395</v>
       </c>
@@ -5146,11 +5338,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="26.25">
+    <row r="134" spans="1:8" ht="26.25">
       <c r="A134" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="B134" s="10"/>
+      <c r="B134" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C134" s="10" t="s">
         <v>33</v>
       </c>
@@ -5167,11 +5361,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="26.25">
+    <row r="135" spans="1:8" ht="26.25">
       <c r="A135" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="B135" s="10"/>
+      <c r="B135" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C135" s="10" t="s">
         <v>404</v>
       </c>
@@ -5188,11 +5384,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="39">
+    <row r="136" spans="1:8" ht="39">
       <c r="A136" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="B136" s="10"/>
+      <c r="B136" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C136" s="10" t="s">
         <v>408</v>
       </c>
@@ -5209,11 +5407,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="26.25">
+    <row r="137" spans="1:8" ht="26.25">
       <c r="A137" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="B137" s="10"/>
+      <c r="B137" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C137" s="10" t="s">
         <v>408</v>
       </c>
@@ -5230,11 +5430,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="26.25">
+    <row r="138" spans="1:8" ht="26.25">
       <c r="A138" s="10" t="s">
         <v>414</v>
       </c>
-      <c r="B138" s="10"/>
+      <c r="B138" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C138" s="10" t="s">
         <v>408</v>
       </c>
@@ -5251,160 +5453,447 @@
         <v>8</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
-      <c r="A139" s="7"/>
-      <c r="B139" s="7"/>
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-      <c r="E139" s="7"/>
-      <c r="F139" s="7"/>
-      <c r="G139" s="7"/>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" s="7"/>
-      <c r="B140" s="7"/>
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-      <c r="E140" s="7"/>
-      <c r="F140" s="7"/>
-      <c r="G140" s="7"/>
-    </row>
-    <row r="141" spans="1:7">
-      <c r="A141" s="7"/>
-      <c r="B141" s="7"/>
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-      <c r="E141" s="7"/>
-      <c r="F141" s="7"/>
-      <c r="G141" s="7"/>
-    </row>
-    <row r="142" spans="1:7">
-      <c r="A142" s="7"/>
-      <c r="B142" s="7"/>
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
-      <c r="F142" s="7"/>
-      <c r="G142" s="7"/>
-    </row>
-    <row r="143" spans="1:7">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-      <c r="E143" s="7"/>
-      <c r="F143" s="7"/>
-      <c r="G143" s="7"/>
-    </row>
-    <row r="144" spans="1:7">
-      <c r="A144" s="7"/>
-      <c r="B144" s="7"/>
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
-      <c r="E144" s="7"/>
-      <c r="F144" s="7"/>
-      <c r="G144" s="7"/>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="7"/>
-      <c r="B145" s="7"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
-      <c r="G145" s="7"/>
-    </row>
-    <row r="146" spans="1:7">
-      <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="7"/>
-      <c r="F146" s="7"/>
-      <c r="G146" s="7"/>
-    </row>
-    <row r="147" spans="1:7">
-      <c r="A147" s="7"/>
-      <c r="B147" s="7"/>
-      <c r="C147" s="7"/>
-      <c r="D147" s="7"/>
-      <c r="E147" s="7"/>
-      <c r="F147" s="7"/>
-      <c r="G147" s="7"/>
-    </row>
-    <row r="148" spans="1:7">
-      <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
-      <c r="C148" s="7"/>
-      <c r="D148" s="7"/>
-      <c r="E148" s="7"/>
-      <c r="F148" s="7"/>
-      <c r="G148" s="7"/>
-    </row>
-    <row r="149" spans="1:7">
-      <c r="A149" s="7"/>
-      <c r="B149" s="7"/>
-      <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
-      <c r="G149" s="7"/>
-    </row>
-    <row r="150" spans="1:7">
-      <c r="A150" s="7"/>
-      <c r="B150" s="7"/>
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-      <c r="E150" s="7"/>
-      <c r="F150" s="7"/>
-      <c r="G150" s="7"/>
-    </row>
-    <row r="151" spans="1:7">
-      <c r="A151" s="7"/>
-      <c r="B151" s="7"/>
-      <c r="C151" s="7"/>
-      <c r="D151" s="7"/>
-      <c r="E151" s="7"/>
-      <c r="F151" s="7"/>
-      <c r="G151" s="7"/>
-    </row>
-    <row r="152" spans="1:7">
-      <c r="A152" s="7"/>
-      <c r="B152" s="7"/>
-      <c r="C152" s="7"/>
-      <c r="D152" s="7"/>
-      <c r="E152" s="7"/>
-      <c r="F152" s="7"/>
-      <c r="G152" s="7"/>
-    </row>
-    <row r="153" spans="1:7">
-      <c r="A153" s="7"/>
-      <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
-      <c r="D153" s="7"/>
-      <c r="E153" s="7"/>
-      <c r="F153" s="7"/>
-      <c r="G153" s="7"/>
-    </row>
-    <row r="154" spans="1:7">
-      <c r="A154" s="7"/>
-      <c r="B154" s="7"/>
-      <c r="C154" s="7"/>
-      <c r="D154" s="7"/>
-      <c r="E154" s="7"/>
-      <c r="F154" s="7"/>
-      <c r="G154" s="7"/>
-    </row>
-    <row r="155" spans="1:7">
-      <c r="A155" s="7"/>
-      <c r="B155" s="7"/>
-      <c r="C155" s="7"/>
-      <c r="D155" s="7"/>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7"/>
-      <c r="G155" s="7"/>
-    </row>
-    <row r="156" spans="1:7">
+    <row r="139" spans="1:8" ht="60">
+      <c r="A139" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D139" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E139" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="F139" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="G139" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H139" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" ht="90">
+      <c r="A140" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D140" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E140" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="F140" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="G140" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H140" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" ht="105">
+      <c r="A141" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D141" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E141" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="F141" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="G141" s="10"/>
+      <c r="H141" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" ht="60">
+      <c r="A142" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C142" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D142" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E142" s="19" t="s">
+        <v>525</v>
+      </c>
+      <c r="F142" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="G142" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H142" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="45">
+      <c r="A143" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C143" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D143" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E143" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="F143" s="19" t="s">
+        <v>528</v>
+      </c>
+      <c r="G143" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H143" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="60">
+      <c r="A144" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="B144" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D144" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E144" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="F144" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="G144" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H144" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="105">
+      <c r="A145" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="B145" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E145" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="F145" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="G145" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H145" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="60">
+      <c r="A146" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="B146" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E146" s="19" t="s">
+        <v>539</v>
+      </c>
+      <c r="F146" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="G146" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H146" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="60">
+      <c r="A147" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="B147" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E147" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="F147" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="G147" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H147" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="60">
+      <c r="A148" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D148" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E148" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="F148" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="G148" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H148" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="45">
+      <c r="A149" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E149" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="F149" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="G149" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H149" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="45">
+      <c r="A150" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E150" s="19" t="s">
+        <v>546</v>
+      </c>
+      <c r="F150" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="G150" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H150" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="45">
+      <c r="A151" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D151" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E151" s="19" t="s">
+        <v>547</v>
+      </c>
+      <c r="F151" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="G151" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H151" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" ht="45">
+      <c r="A152" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D152" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E152" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="F152" s="19" t="s">
+        <v>550</v>
+      </c>
+      <c r="G152" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H152" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" ht="30">
+      <c r="A153" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="B153" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" t="s">
+        <v>464</v>
+      </c>
+      <c r="D153" t="s">
+        <v>10</v>
+      </c>
+      <c r="E153" s="22" t="s">
+        <v>558</v>
+      </c>
+      <c r="F153" s="22" t="s">
+        <v>559</v>
+      </c>
+      <c r="G153" t="s">
+        <v>8</v>
+      </c>
+      <c r="H153" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" ht="45">
+      <c r="A154" s="7" t="s">
+        <v>562</v>
+      </c>
+      <c r="B154" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" t="s">
+        <v>464</v>
+      </c>
+      <c r="D154" t="s">
+        <v>10</v>
+      </c>
+      <c r="E154" s="22" t="s">
+        <v>564</v>
+      </c>
+      <c r="F154" s="22" t="s">
+        <v>560</v>
+      </c>
+      <c r="G154" t="s">
+        <v>8</v>
+      </c>
+      <c r="H154" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="B155" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" t="s">
+        <v>464</v>
+      </c>
+      <c r="D155" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="F155" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="G155" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H155" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
       <c r="A156" s="7"/>
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
@@ -5412,8 +5901,9 @@
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
       <c r="G156" s="7"/>
-    </row>
-    <row r="157" spans="1:7">
+      <c r="H156" s="10"/>
+    </row>
+    <row r="157" spans="1:8">
       <c r="A157" s="7"/>
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
@@ -5421,8 +5911,9 @@
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
       <c r="G157" s="7"/>
-    </row>
-    <row r="158" spans="1:7">
+      <c r="H157" s="10"/>
+    </row>
+    <row r="158" spans="1:8">
       <c r="A158" s="7"/>
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
@@ -5430,8 +5921,9 @@
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
       <c r="G158" s="7"/>
-    </row>
-    <row r="159" spans="1:7">
+      <c r="H158" s="10"/>
+    </row>
+    <row r="159" spans="1:8">
       <c r="A159" s="7"/>
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
@@ -5439,8 +5931,9 @@
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="7"/>
-    </row>
-    <row r="160" spans="1:7">
+      <c r="H159" s="10"/>
+    </row>
+    <row r="160" spans="1:8">
       <c r="A160" s="7"/>
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
@@ -5448,8 +5941,9 @@
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
       <c r="G160" s="7"/>
-    </row>
-    <row r="161" spans="1:7">
+      <c r="H160" s="10"/>
+    </row>
+    <row r="161" spans="1:8">
       <c r="A161" s="7"/>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
@@ -5457,8 +5951,9 @@
       <c r="E161" s="7"/>
       <c r="F161" s="7"/>
       <c r="G161" s="7"/>
-    </row>
-    <row r="162" spans="1:7">
+      <c r="H161" s="10"/>
+    </row>
+    <row r="162" spans="1:8">
       <c r="A162" s="7"/>
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
@@ -5466,8 +5961,9 @@
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
       <c r="G162" s="7"/>
-    </row>
-    <row r="163" spans="1:7">
+      <c r="H162" s="10"/>
+    </row>
+    <row r="163" spans="1:8">
       <c r="A163" s="7"/>
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
@@ -5475,8 +5971,9 @@
       <c r="E163" s="7"/>
       <c r="F163" s="7"/>
       <c r="G163" s="7"/>
-    </row>
-    <row r="164" spans="1:7">
+      <c r="H163" s="10"/>
+    </row>
+    <row r="164" spans="1:8">
       <c r="A164" s="7"/>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
@@ -5484,8 +5981,9 @@
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
       <c r="G164" s="7"/>
-    </row>
-    <row r="165" spans="1:7">
+      <c r="H164" s="10"/>
+    </row>
+    <row r="165" spans="1:8">
       <c r="A165" s="7"/>
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
@@ -5493,8 +5991,9 @@
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
       <c r="G165" s="7"/>
-    </row>
-    <row r="166" spans="1:7">
+      <c r="H165" s="10"/>
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" s="7"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -5502,8 +6001,9 @@
       <c r="E166" s="7"/>
       <c r="F166" s="7"/>
       <c r="G166" s="7"/>
-    </row>
-    <row r="167" spans="1:7">
+      <c r="H166" s="10"/>
+    </row>
+    <row r="167" spans="1:8">
       <c r="A167" s="7"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -5511,8 +6011,9 @@
       <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
-    </row>
-    <row r="168" spans="1:7">
+      <c r="H167" s="10"/>
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" s="7"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -5520,8 +6021,9 @@
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="7"/>
-    </row>
-    <row r="169" spans="1:7">
+      <c r="H168" s="10"/>
+    </row>
+    <row r="169" spans="1:8">
       <c r="A169" s="7"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -5529,8 +6031,9 @@
       <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="7"/>
-    </row>
-    <row r="170" spans="1:7">
+      <c r="H169" s="10"/>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" s="7"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -5538,8 +6041,9 @@
       <c r="E170" s="7"/>
       <c r="F170" s="7"/>
       <c r="G170" s="7"/>
-    </row>
-    <row r="171" spans="1:7">
+      <c r="H170" s="10"/>
+    </row>
+    <row r="171" spans="1:8">
       <c r="A171" s="7"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -5547,8 +6051,9 @@
       <c r="E171" s="7"/>
       <c r="F171" s="7"/>
       <c r="G171" s="7"/>
-    </row>
-    <row r="172" spans="1:7">
+      <c r="H171" s="10"/>
+    </row>
+    <row r="172" spans="1:8">
       <c r="A172" s="7"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -5556,8 +6061,9 @@
       <c r="E172" s="7"/>
       <c r="F172" s="7"/>
       <c r="G172" s="7"/>
-    </row>
-    <row r="173" spans="1:7">
+      <c r="H172" s="10"/>
+    </row>
+    <row r="173" spans="1:8">
       <c r="A173" s="7"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -5565,8 +6071,9 @@
       <c r="E173" s="7"/>
       <c r="F173" s="7"/>
       <c r="G173" s="7"/>
-    </row>
-    <row r="174" spans="1:7">
+      <c r="H173" s="10"/>
+    </row>
+    <row r="174" spans="1:8">
       <c r="A174" s="7"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -5574,8 +6081,9 @@
       <c r="E174" s="7"/>
       <c r="F174" s="7"/>
       <c r="G174" s="7"/>
-    </row>
-    <row r="175" spans="1:7">
+      <c r="H174" s="10"/>
+    </row>
+    <row r="175" spans="1:8">
       <c r="A175" s="7"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -5583,8 +6091,9 @@
       <c r="E175" s="7"/>
       <c r="F175" s="7"/>
       <c r="G175" s="7"/>
-    </row>
-    <row r="176" spans="1:7">
+      <c r="H175" s="10"/>
+    </row>
+    <row r="176" spans="1:8">
       <c r="A176" s="7"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -5592,8 +6101,9 @@
       <c r="E176" s="7"/>
       <c r="F176" s="7"/>
       <c r="G176" s="7"/>
-    </row>
-    <row r="177" spans="1:7">
+      <c r="H176" s="10"/>
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" s="7"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -5601,8 +6111,9 @@
       <c r="E177" s="7"/>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
-    </row>
-    <row r="178" spans="1:7">
+      <c r="H177" s="10"/>
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" s="7"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -5610,8 +6121,9 @@
       <c r="E178" s="7"/>
       <c r="F178" s="7"/>
       <c r="G178" s="7"/>
-    </row>
-    <row r="179" spans="1:7">
+      <c r="H178" s="10"/>
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" s="7"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -5619,8 +6131,9 @@
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
       <c r="G179" s="7"/>
-    </row>
-    <row r="180" spans="1:7">
+      <c r="H179" s="10"/>
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" s="7"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -5628,8 +6141,9 @@
       <c r="E180" s="7"/>
       <c r="F180" s="7"/>
       <c r="G180" s="7"/>
-    </row>
-    <row r="181" spans="1:7">
+      <c r="H180" s="10"/>
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" s="7"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -5637,8 +6151,9 @@
       <c r="E181" s="7"/>
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
-    </row>
-    <row r="182" spans="1:7">
+      <c r="H181" s="10"/>
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" s="7"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -5646,8 +6161,9 @@
       <c r="E182" s="7"/>
       <c r="F182" s="7"/>
       <c r="G182" s="7"/>
-    </row>
-    <row r="183" spans="1:7">
+      <c r="H182" s="10"/>
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" s="7"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -5655,8 +6171,9 @@
       <c r="E183" s="7"/>
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
-    </row>
-    <row r="184" spans="1:7">
+      <c r="H183" s="10"/>
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184" s="7"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -5664,8 +6181,9 @@
       <c r="E184" s="7"/>
       <c r="F184" s="7"/>
       <c r="G184" s="7"/>
-    </row>
-    <row r="185" spans="1:7">
+      <c r="H184" s="10"/>
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" s="7"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -5673,8 +6191,9 @@
       <c r="E185" s="7"/>
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
-    </row>
-    <row r="186" spans="1:7">
+      <c r="H185" s="10"/>
+    </row>
+    <row r="186" spans="1:8">
       <c r="A186" s="7"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -5682,8 +6201,9 @@
       <c r="E186" s="7"/>
       <c r="F186" s="7"/>
       <c r="G186" s="7"/>
-    </row>
-    <row r="187" spans="1:7">
+      <c r="H186" s="10"/>
+    </row>
+    <row r="187" spans="1:8">
       <c r="A187" s="7"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -5691,8 +6211,9 @@
       <c r="E187" s="7"/>
       <c r="F187" s="7"/>
       <c r="G187" s="7"/>
-    </row>
-    <row r="188" spans="1:7">
+      <c r="H187" s="10"/>
+    </row>
+    <row r="188" spans="1:8">
       <c r="A188" s="7"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -5700,8 +6221,9 @@
       <c r="E188" s="7"/>
       <c r="F188" s="7"/>
       <c r="G188" s="7"/>
-    </row>
-    <row r="189" spans="1:7">
+      <c r="H188" s="10"/>
+    </row>
+    <row r="189" spans="1:8">
       <c r="A189" s="7"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -5709,8 +6231,9 @@
       <c r="E189" s="7"/>
       <c r="F189" s="7"/>
       <c r="G189" s="7"/>
-    </row>
-    <row r="190" spans="1:7">
+      <c r="H189" s="10"/>
+    </row>
+    <row r="190" spans="1:8">
       <c r="A190" s="7"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -5718,8 +6241,9 @@
       <c r="E190" s="7"/>
       <c r="F190" s="7"/>
       <c r="G190" s="7"/>
-    </row>
-    <row r="191" spans="1:7">
+      <c r="H190" s="10"/>
+    </row>
+    <row r="191" spans="1:8">
       <c r="A191" s="7"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -5727,8 +6251,9 @@
       <c r="E191" s="7"/>
       <c r="F191" s="7"/>
       <c r="G191" s="7"/>
-    </row>
-    <row r="192" spans="1:7">
+      <c r="H191" s="10"/>
+    </row>
+    <row r="192" spans="1:8">
       <c r="A192" s="7"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -5736,6 +6261,7 @@
       <c r="E192" s="7"/>
       <c r="F192" s="7"/>
       <c r="G192" s="7"/>
+      <c r="H192" s="10"/>
     </row>
     <row r="193" spans="1:7">
       <c r="A193" s="7"/>
@@ -8979,17 +9505,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B133 B139:B552">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B138 B156:B552">
       <formula1>"Admin, IDA, Partner Mgmt, Pre Registration, Registration Client, Registration Processor, Resident Services"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D299">
       <formula1>"Acceptance, Functional, Smoke, Security, Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G299">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H139:H154 G2:G299">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B134:B138">
-      <formula1>"Admin, IDA, Partner Mgmt, Registration Client, Registration Processor, Resident Services"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B139:B155">
+      <formula1>"Admin, Credential Services, IDA, Partner Mgmt, Pre Registration, Registration Client, Registration Processor, Resident Services"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9001,7 +9527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Testcases for story 1.1.5 is uploaded
</commit_message>
<xml_diff>
--- a/Master-functional-testcases/Pre-registration/TC_PreRegistration.xlsx
+++ b/Master-functional-testcases/Pre-registration/TC_PreRegistration.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niyati.Swami\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anushree.N\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Pre-reg" sheetId="1" r:id="rId1"/>
@@ -17,9 +17,9 @@
     <sheet name="1.2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pre-reg'!$A$1:$G$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pre-reg'!$A$1:$I$204</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1393" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="701">
   <si>
     <t xml:space="preserve">TestCase_No </t>
   </si>
@@ -1258,18 +1258,6 @@
     <t>Pre Registration_ UI Test cases_46</t>
   </si>
   <si>
-    <t>Pre Registration_ UI Test cases_47</t>
-  </si>
-  <si>
-    <t>Pre Registration_ UI Test cases_48</t>
-  </si>
-  <si>
-    <t>Pre Registration_ UI Test cases_49</t>
-  </si>
-  <si>
-    <t>Pre Registration_ UI Test cases_50</t>
-  </si>
-  <si>
     <t>Smoke</t>
   </si>
   <si>
@@ -1784,13 +1772,428 @@
   </si>
   <si>
     <t>The API call should be made through pre-reg not direct to masterData</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_01</t>
+  </si>
+  <si>
+    <t>preview page</t>
+  </si>
+  <si>
+    <t>To verify that preview page displays the location names .</t>
+  </si>
+  <si>
+    <t>Preview page should display the location names as per the selected.</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_02</t>
+  </si>
+  <si>
+    <t>To verify that location codes are not displayed in the preview page.</t>
+  </si>
+  <si>
+    <t>Location codes should not be  displayed in the preview page rather it should display respective location names.</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_03</t>
+  </si>
+  <si>
+    <t>To verify that the displayed locations in preview page are same that of selected locations in the dropdown while creation.</t>
+  </si>
+  <si>
+    <t>The displayed locations in preview page should be  same as  that of selected locations in the dropdown in demographic page.</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_04</t>
+  </si>
+  <si>
+    <t>To verify that location names are displayed in sequence to that of sequence in  demographic page.</t>
+  </si>
+  <si>
+    <t>Location names should be displayed in sequence to that of sequence in  demographic page or as per location hierarchy.</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_05</t>
+  </si>
+  <si>
+    <t>To verify that any modication or changes made are updated and  are reflected same in preview page.</t>
+  </si>
+  <si>
+    <t>Any modication or changes made should be updated and  must reflect same in preview page.</t>
+  </si>
+  <si>
+    <t>Pre Reg_preview_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that same location names are  fetched in regclient when PRID is synced </t>
+  </si>
+  <si>
+    <t>Same location names need to be   fetched in regclient when PRID is synced .</t>
+  </si>
+  <si>
+    <t>MOSIP-11299</t>
+  </si>
+  <si>
+    <t>MOSIP-11300</t>
+  </si>
+  <si>
+    <t>Pre Reg_repository_1</t>
+  </si>
+  <si>
+    <t>Git Repository</t>
+  </si>
+  <si>
+    <t>To Verify that new GitHub repository is created other than the centralized repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Their should be separate repository for Pre - Registration UI </t>
+  </si>
+  <si>
+    <t>Pre Reg_repository_2</t>
+  </si>
+  <si>
+    <t>To verify that all the active branches are present in the new GitHub repository as that of centralized repository.</t>
+  </si>
+  <si>
+    <t>It should include all the active branches as same as centralized repository.</t>
+  </si>
+  <si>
+    <t>Pre Reg_repository_3</t>
+  </si>
+  <si>
+    <t>To verify that the cloning of new repository  to local system should work correctly.</t>
+  </si>
+  <si>
+    <t>It should work as expected.</t>
+  </si>
+  <si>
+    <t>Pre Reg_repository_4</t>
+  </si>
+  <si>
+    <t>To verify that All the code commits are  happening in respective repositories.</t>
+  </si>
+  <si>
+    <t>changes made as per the requirement should get reflected in the respective repository.</t>
+  </si>
+  <si>
+    <t>Pre Reg_repository_5</t>
+  </si>
+  <si>
+    <t>To verify that pre reg UI is working as expected .</t>
+  </si>
+  <si>
+    <t>Creation of new repository should not affect the current pre reg UI.</t>
+  </si>
+  <si>
+    <t>MOSIP-11496</t>
+  </si>
+  <si>
+    <t>To verfiy the document category shown to be uploaded on document  page for Adult_foreigner</t>
+  </si>
+  <si>
+    <t>The user should get the number of document mapped with applicant type and user should be able to uplaod the doc and proceed further</t>
+  </si>
+  <si>
+    <t>To verfiy the document category shown to be uploaded on document  page for Adult_NonForeigner</t>
+  </si>
+  <si>
+    <t>To verfiy the document category shown to be uploaded on document  page for Minor_foreigner</t>
+  </si>
+  <si>
+    <t>To verfiy the document category shown to be uploaded on document  page for Minor_Non-foreigner</t>
+  </si>
+  <si>
+    <t>MOSIP-10946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book appointment </t>
+  </si>
+  <si>
+    <t>To verify that if we search with country you should be able to see the count of registration center.</t>
+  </si>
+  <si>
+    <t>The user should be able to view the centers based on location selected.</t>
+  </si>
+  <si>
+    <t>To verify that on selecting the location one should be able to see a pagination ,number of centers per page we select.</t>
+  </si>
+  <si>
+    <t>To validate that on selecting the location one should be able to see a pagination ,number of centers per page we select. And check if all centers are displayed based on our selection.</t>
+  </si>
+  <si>
+    <t>To verify that  one can navigate to different records and should be able to choose records per page.</t>
+  </si>
+  <si>
+    <t>User should be able to navigate to different pages as per his convinience and should as be able to choose records per page.</t>
+  </si>
+  <si>
+    <t>To verify that previous page is disabled if we are in  second page.</t>
+  </si>
+  <si>
+    <t>Other than the current page all other pages opened previous should be disabled.</t>
+  </si>
+  <si>
+    <t>To verify that the user must not be able to select two centers at a time.</t>
+  </si>
+  <si>
+    <t>User should not be allowed to choose two registration center at a time.</t>
+  </si>
+  <si>
+    <t>To verify that all data is fetched when PRID is synced to reg client</t>
+  </si>
+  <si>
+    <t>All data of User should be fetched when PRID is synced in reg client.</t>
+  </si>
+  <si>
+    <t>MOSIP-11297</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_1</t>
+  </si>
+  <si>
+    <t>Demographic page</t>
+  </si>
+  <si>
+    <t>To verify that fields of Pre-Reg are customized  based on the type of user registering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fields of Pre-Reg should be  customized  based on the type of user registering.</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_2</t>
+  </si>
+  <si>
+    <t>To verify that if the age of a resident is more than or equal to 60 then they should be considered as a senior citizen and must be asked to fillin the proof of age field.</t>
+  </si>
+  <si>
+    <t>It should display a cutomized fields based on the resident age</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_3</t>
+  </si>
+  <si>
+    <t>To verify that if the age of a resident is 10 years or less than that should be considered as child and must be asked to fillin proof of relation field (parent or guardian)</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_4</t>
+  </si>
+  <si>
+    <t>To verify that if the age of resident is 0 or less than that should throw an appropriate error message "Enter valid DOB".</t>
+  </si>
+  <si>
+    <t>Should throw an error message</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_5</t>
+  </si>
+  <si>
+    <t>To verify that if the age of the resident is more than 100 must show the error message as "Invalid DOB"</t>
+  </si>
+  <si>
+    <t>MOSIP-10847</t>
+  </si>
+  <si>
+    <t>To verify that  book appointment page UI should display location hierarchy in correct order</t>
+  </si>
+  <si>
+    <t>Book appointment page UI should display location hierarchy in correct order(ex:World&gt;&gt;country&gt;&gt;province&gt;&gt;city&gt;&gt;barangey&gt;&gt;postal code.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that registration centers are display with respect to the location selected from the  drop down </t>
+  </si>
+  <si>
+    <t>Registration centers should be  displayed with respect to the location selected from the  drop down.</t>
+  </si>
+  <si>
+    <t>To verify  that all registration center which are mapped are shown as an option when user select particular location.</t>
+  </si>
+  <si>
+    <t>Registration center which are mapped should be  shown as an option when user selects  particular location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that changes are reflected when the user modifies his data.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Any Changes made should get reflected when the user modifies his data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that registration centers mapped to the location should be displayed correctly after the changes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Registration centers mapped to the location should be displayed correctly even after making changes. </t>
+  </si>
+  <si>
+    <t>To verify  that  the location hierarchy  levels are not shown after selecting a location( ex: if city is choosen it shouldn't ask user to enter postal code)</t>
+  </si>
+  <si>
+    <t>The location hierarchy  levels should  not be  shown after selecting a particular location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To verify that all details of user are  fetched in regclient when PRID is synced </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All  details of user should be  fetched in regclient when PRID is synced. </t>
+  </si>
+  <si>
+    <t>To verify  the user scetion after First attempt of login in pre-reg</t>
+  </si>
+  <si>
+    <t>No value should be saved inside the user section under pre-reg in keycloak after first login</t>
+  </si>
+  <si>
+    <t>Verify from where the issuer call  is coming</t>
+  </si>
+  <si>
+    <t>The issuer should be from Keycloak and come from OTP transaction table</t>
+  </si>
+  <si>
+    <t>verify that where the email and OTP is saved in OTP Trnsaction table</t>
+  </si>
+  <si>
+    <t>There should be a specified column from where the data is saved</t>
+  </si>
+  <si>
+    <t>MOSIP-9961</t>
+  </si>
+  <si>
+    <t>MOSIP-10959</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_6</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_7</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_8</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_9</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_10</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_11</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_12</t>
+  </si>
+  <si>
+    <t>Pre Reg_Demo_13</t>
+  </si>
+  <si>
+    <t>MOSIP-10958</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_25</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_26</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_27</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_28</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_29</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_30</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_31</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_32</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_33</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_34</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_35</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_36</t>
+  </si>
+  <si>
+    <t>Pre Registration_Book Appointment_37</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_28</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_29</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_30</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_31</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_32</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_33</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_34</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_35</t>
+  </si>
+  <si>
+    <t>Pre Registration_Document_36</t>
+  </si>
+  <si>
+    <t>PreReg_Login_11</t>
+  </si>
+  <si>
+    <t>Registration Client_Login_12</t>
+  </si>
+  <si>
+    <t>Registration Client_Login_13</t>
+  </si>
+  <si>
+    <t>Registration Client_Login_14</t>
+  </si>
+  <si>
+    <t>Pre Registration_Other_2</t>
+  </si>
+  <si>
+    <t>Pre Registration_Other_3</t>
+  </si>
+  <si>
+    <t>Pre Registration_Other_4</t>
+  </si>
+  <si>
+    <t>Pre Registration_Other_5</t>
+  </si>
+  <si>
+    <t>Pre Registration_ UI Test cases_01</t>
+  </si>
+  <si>
+    <t>Pre Registration_ UI Test cases_02</t>
+  </si>
+  <si>
+    <t>Pre Registration_ UI Test cases_03</t>
+  </si>
+  <si>
+    <t>Pre Registration_ UI Test cases_04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1827,6 +2230,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1901,7 +2310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1963,6 +2372,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2243,10 +2662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H552"/>
+  <dimension ref="A1:I552"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H159" sqref="A1:XFD1048576"/>
+      <selection activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2283,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="89.25">
@@ -2435,7 +2854,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
@@ -2523,7 +2942,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>34</v>
@@ -2546,7 +2965,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>36</v>
@@ -2707,7 +3126,7 @@
         <v>49</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>50</v>
@@ -2755,7 +3174,7 @@
         <v>49</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>54</v>
@@ -3569,7 +3988,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="38.25">
+    <row r="57" spans="1:7" ht="51">
       <c r="A57" s="7" t="s">
         <v>294</v>
       </c>
@@ -3626,7 +4045,7 @@
         <v>12</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>125</v>
@@ -3649,7 +4068,7 @@
         <v>12</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>127</v>
@@ -3672,7 +4091,7 @@
         <v>12</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>129</v>
@@ -3718,7 +4137,7 @@
         <v>12</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>133</v>
@@ -3764,7 +4183,7 @@
         <v>12</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>136</v>
@@ -3856,7 +4275,7 @@
         <v>137</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>144</v>
@@ -3902,7 +4321,7 @@
         <v>137</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>148</v>
@@ -4077,13 +4496,13 @@
     </row>
     <row r="79" spans="1:7" ht="38.25">
       <c r="A79" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>10</v>
@@ -4100,13 +4519,13 @@
     </row>
     <row r="80" spans="1:7" ht="25.5">
       <c r="A80" s="7" t="s">
-        <v>399</v>
+        <v>693</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>10</v>
@@ -4123,13 +4542,13 @@
     </row>
     <row r="81" spans="1:7" ht="38.25">
       <c r="A81" s="7" t="s">
-        <v>399</v>
+        <v>694</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>10</v>
@@ -4146,13 +4565,13 @@
     </row>
     <row r="82" spans="1:7" ht="25.5">
       <c r="A82" s="7" t="s">
-        <v>399</v>
+        <v>695</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>10</v>
@@ -4169,13 +4588,13 @@
     </row>
     <row r="83" spans="1:7" ht="25.5">
       <c r="A83" s="7" t="s">
-        <v>399</v>
+        <v>696</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="5" t="s">
@@ -4199,7 +4618,7 @@
         <v>180</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>181</v>
@@ -4222,7 +4641,7 @@
         <v>180</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>183</v>
@@ -4245,7 +4664,7 @@
         <v>180</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>185</v>
@@ -4314,7 +4733,7 @@
         <v>180</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>190</v>
@@ -4659,7 +5078,7 @@
         <v>180</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>218</v>
@@ -4682,7 +5101,7 @@
         <v>180</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>220</v>
@@ -4705,7 +5124,7 @@
         <v>180</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E106" s="3" t="s">
         <v>222</v>
@@ -4728,7 +5147,7 @@
         <v>180</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E107" s="3" t="s">
         <v>224</v>
@@ -4751,7 +5170,7 @@
         <v>180</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E108" s="3" t="s">
         <v>226</v>
@@ -4774,7 +5193,7 @@
         <v>180</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E109" s="3" t="s">
         <v>228</v>
@@ -4797,7 +5216,7 @@
         <v>180</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E110" s="3" t="s">
         <v>153</v>
@@ -4820,7 +5239,7 @@
         <v>180</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E111" s="3" t="s">
         <v>231</v>
@@ -4843,7 +5262,7 @@
         <v>180</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E112" s="3" t="s">
         <v>233</v>
@@ -5248,7 +5667,7 @@
     </row>
     <row r="130" spans="1:8" ht="25.5">
       <c r="A130" s="7" t="s">
-        <v>392</v>
+        <v>697</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>11</v>
@@ -5257,7 +5676,7 @@
         <v>171</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E130" s="3" t="s">
         <v>172</v>
@@ -5271,7 +5690,7 @@
     </row>
     <row r="131" spans="1:8" ht="25.5">
       <c r="A131" s="7" t="s">
-        <v>393</v>
+        <v>698</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>11</v>
@@ -5280,7 +5699,7 @@
         <v>171</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E131" s="3" t="s">
         <v>174</v>
@@ -5294,7 +5713,7 @@
     </row>
     <row r="132" spans="1:8" ht="25.5">
       <c r="A132" s="7" t="s">
-        <v>394</v>
+        <v>699</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>11</v>
@@ -5317,7 +5736,7 @@
     </row>
     <row r="133" spans="1:8" ht="51">
       <c r="A133" s="7" t="s">
-        <v>395</v>
+        <v>700</v>
       </c>
       <c r="B133" s="7" t="s">
         <v>11</v>
@@ -5340,7 +5759,7 @@
     </row>
     <row r="134" spans="1:8" ht="26.25">
       <c r="A134" s="10" t="s">
-        <v>400</v>
+        <v>689</v>
       </c>
       <c r="B134" s="7" t="s">
         <v>11</v>
@@ -5352,10 +5771,10 @@
         <v>10</v>
       </c>
       <c r="E134" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F134" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G134" s="10" t="s">
         <v>8</v>
@@ -5363,22 +5782,22 @@
     </row>
     <row r="135" spans="1:8" ht="26.25">
       <c r="A135" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B135" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C135" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E135" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F135" s="11" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>8</v>
@@ -5386,22 +5805,22 @@
     </row>
     <row r="136" spans="1:8" ht="39">
       <c r="A136" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B136" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C136" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D136" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E136" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G136" s="10" t="s">
         <v>8</v>
@@ -5409,22 +5828,22 @@
     </row>
     <row r="137" spans="1:8" ht="26.25">
       <c r="A137" s="10" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B137" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C137" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="D137" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="D137" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E137" s="11" t="s">
-        <v>412</v>
-      </c>
       <c r="F137" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G137" s="10" t="s">
         <v>8</v>
@@ -5432,22 +5851,22 @@
     </row>
     <row r="138" spans="1:8" ht="26.25">
       <c r="A138" s="10" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B138" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C138" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D138" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E138" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F138" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G138" s="10" t="s">
         <v>8</v>
@@ -5455,7 +5874,7 @@
     </row>
     <row r="139" spans="1:8" ht="60">
       <c r="A139" s="7" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B139" s="10" t="s">
         <v>11</v>
@@ -5467,10 +5886,10 @@
         <v>10</v>
       </c>
       <c r="E139" s="19" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="F139" s="19" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="G139" s="10" t="s">
         <v>8</v>
@@ -5481,7 +5900,7 @@
     </row>
     <row r="140" spans="1:8" ht="90">
       <c r="A140" s="7" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B140" s="10" t="s">
         <v>11</v>
@@ -5493,10 +5912,10 @@
         <v>10</v>
       </c>
       <c r="E140" s="19" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="F140" s="19" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G140" s="10" t="s">
         <v>8</v>
@@ -5507,7 +5926,7 @@
     </row>
     <row r="141" spans="1:8" ht="105">
       <c r="A141" s="7" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B141" s="10" t="s">
         <v>11</v>
@@ -5519,10 +5938,10 @@
         <v>10</v>
       </c>
       <c r="E141" s="19" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F141" s="19" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G141" s="10"/>
       <c r="H141" s="10" t="s">
@@ -5531,7 +5950,7 @@
     </row>
     <row r="142" spans="1:8" ht="60">
       <c r="A142" s="7" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B142" s="10" t="s">
         <v>11</v>
@@ -5543,10 +5962,10 @@
         <v>10</v>
       </c>
       <c r="E142" s="19" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="F142" s="19" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="G142" s="10" t="s">
         <v>8</v>
@@ -5557,7 +5976,7 @@
     </row>
     <row r="143" spans="1:8" ht="45">
       <c r="A143" s="7" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B143" s="10" t="s">
         <v>11</v>
@@ -5569,10 +5988,10 @@
         <v>10</v>
       </c>
       <c r="E143" s="19" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F143" s="19" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="G143" s="10" t="s">
         <v>8</v>
@@ -5583,7 +6002,7 @@
     </row>
     <row r="144" spans="1:8" ht="60">
       <c r="A144" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B144" s="10" t="s">
         <v>11</v>
@@ -5595,10 +6014,10 @@
         <v>10</v>
       </c>
       <c r="E144" s="19" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="F144" s="19" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="G144" s="10" t="s">
         <v>8</v>
@@ -5607,9 +6026,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="105">
+    <row r="145" spans="1:9" ht="105">
       <c r="A145" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B145" s="10" t="s">
         <v>11</v>
@@ -5621,10 +6040,10 @@
         <v>10</v>
       </c>
       <c r="E145" s="19" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F145" s="19" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="G145" s="10" t="s">
         <v>8</v>
@@ -5633,9 +6052,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="60">
+    <row r="146" spans="1:9" ht="60">
       <c r="A146" s="7" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B146" s="10" t="s">
         <v>11</v>
@@ -5647,10 +6066,10 @@
         <v>10</v>
       </c>
       <c r="E146" s="19" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="F146" s="19" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G146" s="10" t="s">
         <v>8</v>
@@ -5659,9 +6078,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="60">
+    <row r="147" spans="1:9" ht="60">
       <c r="A147" s="7" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B147" s="10" t="s">
         <v>11</v>
@@ -5673,10 +6092,10 @@
         <v>10</v>
       </c>
       <c r="E147" s="19" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F147" s="19" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="G147" s="10" t="s">
         <v>8</v>
@@ -5685,9 +6104,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="60">
+    <row r="148" spans="1:9" ht="60">
       <c r="A148" s="7" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B148" s="10" t="s">
         <v>11</v>
@@ -5699,10 +6118,10 @@
         <v>10</v>
       </c>
       <c r="E148" s="19" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="F148" s="19" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="G148" s="10" t="s">
         <v>8</v>
@@ -5711,9 +6130,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="45">
+    <row r="149" spans="1:9" ht="45">
       <c r="A149" s="7" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B149" s="10" t="s">
         <v>11</v>
@@ -5725,10 +6144,10 @@
         <v>10</v>
       </c>
       <c r="E149" s="19" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F149" s="19" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G149" s="10" t="s">
         <v>8</v>
@@ -5737,9 +6156,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="45">
+    <row r="150" spans="1:9" ht="45">
       <c r="A150" s="7" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B150" s="10" t="s">
         <v>11</v>
@@ -5751,10 +6170,10 @@
         <v>10</v>
       </c>
       <c r="E150" s="19" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F150" s="19" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="G150" s="10" t="s">
         <v>8</v>
@@ -5763,9 +6182,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="45">
+    <row r="151" spans="1:9" ht="45">
       <c r="A151" s="7" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B151" s="10" t="s">
         <v>11</v>
@@ -5777,10 +6196,10 @@
         <v>10</v>
       </c>
       <c r="E151" s="19" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F151" s="19" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="G151" s="10" t="s">
         <v>8</v>
@@ -5789,9 +6208,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="45">
+    <row r="152" spans="1:9" ht="45">
       <c r="A152" s="7" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B152" s="10" t="s">
         <v>11</v>
@@ -5803,10 +6222,10 @@
         <v>10</v>
       </c>
       <c r="E152" s="19" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="F152" s="19" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="G152" s="21" t="s">
         <v>8</v>
@@ -5815,24 +6234,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="30">
+    <row r="153" spans="1:9" ht="30">
       <c r="A153" s="7" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B153" t="s">
         <v>11</v>
       </c>
       <c r="C153" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D153" t="s">
         <v>10</v>
       </c>
       <c r="E153" s="22" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F153" s="22" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="G153" t="s">
         <v>8</v>
@@ -5841,24 +6260,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="45">
+    <row r="154" spans="1:9" ht="45">
       <c r="A154" s="7" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B154" t="s">
         <v>11</v>
       </c>
       <c r="C154" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D154" t="s">
         <v>10</v>
       </c>
       <c r="E154" s="22" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F154" s="22" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="G154" t="s">
         <v>8</v>
@@ -5867,24 +6286,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:9">
       <c r="A155" s="7" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B155" t="s">
         <v>11</v>
       </c>
       <c r="C155" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D155" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E155" s="7" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="G155" s="7" t="s">
         <v>8</v>
@@ -5893,485 +6312,1217 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
-      <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
-      <c r="C156" s="7"/>
-      <c r="D156" s="7"/>
-      <c r="E156" s="7"/>
-      <c r="F156" s="7"/>
-      <c r="G156" s="7"/>
-      <c r="H156" s="10"/>
-    </row>
-    <row r="157" spans="1:8">
-      <c r="A157" s="7"/>
-      <c r="B157" s="7"/>
-      <c r="C157" s="7"/>
-      <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
-      <c r="G157" s="7"/>
-      <c r="H157" s="10"/>
-    </row>
-    <row r="158" spans="1:8">
-      <c r="A158" s="7"/>
-      <c r="B158" s="7"/>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7"/>
-      <c r="F158" s="7"/>
-      <c r="G158" s="7"/>
-      <c r="H158" s="10"/>
-    </row>
-    <row r="159" spans="1:8">
-      <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
-      <c r="C159" s="7"/>
-      <c r="D159" s="7"/>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7"/>
-      <c r="G159" s="7"/>
-      <c r="H159" s="10"/>
-    </row>
-    <row r="160" spans="1:8">
-      <c r="A160" s="7"/>
-      <c r="B160" s="7"/>
-      <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
-      <c r="G160" s="7"/>
-      <c r="H160" s="10"/>
-    </row>
-    <row r="161" spans="1:8">
-      <c r="A161" s="7"/>
-      <c r="B161" s="7"/>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
-      <c r="E161" s="7"/>
-      <c r="F161" s="7"/>
-      <c r="G161" s="7"/>
-      <c r="H161" s="10"/>
-    </row>
-    <row r="162" spans="1:8">
-      <c r="A162" s="7"/>
-      <c r="B162" s="7"/>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="7"/>
-      <c r="F162" s="7"/>
-      <c r="G162" s="7"/>
-      <c r="H162" s="10"/>
-    </row>
-    <row r="163" spans="1:8">
-      <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
-      <c r="C163" s="7"/>
-      <c r="D163" s="7"/>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="7"/>
-      <c r="H163" s="10"/>
-    </row>
-    <row r="164" spans="1:8">
-      <c r="A164" s="7"/>
-      <c r="B164" s="7"/>
-      <c r="C164" s="7"/>
-      <c r="D164" s="7"/>
-      <c r="E164" s="7"/>
-      <c r="F164" s="7"/>
-      <c r="G164" s="7"/>
-      <c r="H164" s="10"/>
-    </row>
-    <row r="165" spans="1:8">
-      <c r="A165" s="7"/>
-      <c r="B165" s="7"/>
-      <c r="C165" s="7"/>
-      <c r="D165" s="7"/>
-      <c r="E165" s="7"/>
-      <c r="F165" s="7"/>
-      <c r="G165" s="7"/>
-      <c r="H165" s="10"/>
-    </row>
-    <row r="166" spans="1:8">
-      <c r="A166" s="7"/>
-      <c r="B166" s="7"/>
-      <c r="C166" s="7"/>
-      <c r="D166" s="7"/>
-      <c r="E166" s="7"/>
-      <c r="F166" s="7"/>
-      <c r="G166" s="7"/>
-      <c r="H166" s="10"/>
-    </row>
-    <row r="167" spans="1:8">
-      <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-      <c r="D167" s="7"/>
-      <c r="E167" s="7"/>
-      <c r="F167" s="7"/>
-      <c r="G167" s="7"/>
-      <c r="H167" s="10"/>
-    </row>
-    <row r="168" spans="1:8">
-      <c r="A168" s="7"/>
-      <c r="B168" s="7"/>
-      <c r="C168" s="7"/>
-      <c r="D168" s="7"/>
-      <c r="E168" s="7"/>
-      <c r="F168" s="7"/>
-      <c r="G168" s="7"/>
-      <c r="H168" s="10"/>
-    </row>
-    <row r="169" spans="1:8">
-      <c r="A169" s="7"/>
-      <c r="B169" s="7"/>
-      <c r="C169" s="7"/>
-      <c r="D169" s="7"/>
-      <c r="E169" s="7"/>
-      <c r="F169" s="7"/>
-      <c r="G169" s="7"/>
-      <c r="H169" s="10"/>
-    </row>
-    <row r="170" spans="1:8">
-      <c r="A170" s="7"/>
-      <c r="B170" s="7"/>
-      <c r="C170" s="7"/>
-      <c r="D170" s="7"/>
-      <c r="E170" s="7"/>
-      <c r="F170" s="7"/>
-      <c r="G170" s="7"/>
-      <c r="H170" s="10"/>
-    </row>
-    <row r="171" spans="1:8">
-      <c r="A171" s="7"/>
-      <c r="B171" s="7"/>
-      <c r="C171" s="7"/>
-      <c r="D171" s="7"/>
-      <c r="E171" s="7"/>
-      <c r="F171" s="7"/>
-      <c r="G171" s="7"/>
-      <c r="H171" s="10"/>
-    </row>
-    <row r="172" spans="1:8">
-      <c r="A172" s="7"/>
-      <c r="B172" s="7"/>
-      <c r="C172" s="7"/>
-      <c r="D172" s="7"/>
-      <c r="E172" s="7"/>
-      <c r="F172" s="7"/>
-      <c r="G172" s="7"/>
-      <c r="H172" s="10"/>
-    </row>
-    <row r="173" spans="1:8">
-      <c r="A173" s="7"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="7"/>
-      <c r="D173" s="7"/>
-      <c r="E173" s="7"/>
-      <c r="F173" s="7"/>
-      <c r="G173" s="7"/>
-      <c r="H173" s="10"/>
-    </row>
-    <row r="174" spans="1:8">
-      <c r="A174" s="7"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="7"/>
-      <c r="D174" s="7"/>
-      <c r="E174" s="7"/>
-      <c r="F174" s="7"/>
-      <c r="G174" s="7"/>
-      <c r="H174" s="10"/>
-    </row>
-    <row r="175" spans="1:8">
-      <c r="A175" s="7"/>
-      <c r="B175" s="7"/>
-      <c r="C175" s="7"/>
-      <c r="D175" s="7"/>
-      <c r="E175" s="7"/>
-      <c r="F175" s="7"/>
-      <c r="G175" s="7"/>
-      <c r="H175" s="10"/>
-    </row>
-    <row r="176" spans="1:8">
-      <c r="A176" s="7"/>
-      <c r="B176" s="7"/>
-      <c r="C176" s="7"/>
-      <c r="D176" s="7"/>
-      <c r="E176" s="7"/>
-      <c r="F176" s="7"/>
-      <c r="G176" s="7"/>
-      <c r="H176" s="10"/>
-    </row>
-    <row r="177" spans="1:8">
-      <c r="A177" s="7"/>
-      <c r="B177" s="7"/>
-      <c r="C177" s="7"/>
-      <c r="D177" s="7"/>
-      <c r="E177" s="7"/>
-      <c r="F177" s="7"/>
-      <c r="G177" s="7"/>
-      <c r="H177" s="10"/>
-    </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="7"/>
-      <c r="B178" s="7"/>
-      <c r="C178" s="7"/>
-      <c r="D178" s="7"/>
-      <c r="E178" s="7"/>
-      <c r="F178" s="7"/>
-      <c r="G178" s="7"/>
-      <c r="H178" s="10"/>
-    </row>
-    <row r="179" spans="1:8">
-      <c r="A179" s="7"/>
-      <c r="B179" s="7"/>
-      <c r="C179" s="7"/>
-      <c r="D179" s="7"/>
-      <c r="E179" s="7"/>
-      <c r="F179" s="7"/>
-      <c r="G179" s="7"/>
-      <c r="H179" s="10"/>
-    </row>
-    <row r="180" spans="1:8">
-      <c r="A180" s="7"/>
-      <c r="B180" s="7"/>
-      <c r="C180" s="7"/>
-      <c r="D180" s="7"/>
-      <c r="E180" s="7"/>
-      <c r="F180" s="7"/>
-      <c r="G180" s="7"/>
-      <c r="H180" s="10"/>
-    </row>
-    <row r="181" spans="1:8">
-      <c r="A181" s="7"/>
-      <c r="B181" s="7"/>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="7"/>
-      <c r="F181" s="7"/>
-      <c r="G181" s="7"/>
-      <c r="H181" s="10"/>
-    </row>
-    <row r="182" spans="1:8">
-      <c r="A182" s="7"/>
-      <c r="B182" s="7"/>
-      <c r="C182" s="7"/>
-      <c r="D182" s="7"/>
-      <c r="E182" s="7"/>
-      <c r="F182" s="7"/>
-      <c r="G182" s="7"/>
-      <c r="H182" s="10"/>
-    </row>
-    <row r="183" spans="1:8">
-      <c r="A183" s="7"/>
-      <c r="B183" s="7"/>
-      <c r="C183" s="7"/>
-      <c r="D183" s="7"/>
-      <c r="E183" s="7"/>
-      <c r="F183" s="7"/>
-      <c r="G183" s="7"/>
-      <c r="H183" s="10"/>
-    </row>
-    <row r="184" spans="1:8">
-      <c r="A184" s="7"/>
-      <c r="B184" s="7"/>
-      <c r="C184" s="7"/>
-      <c r="D184" s="7"/>
-      <c r="E184" s="7"/>
-      <c r="F184" s="7"/>
-      <c r="G184" s="7"/>
-      <c r="H184" s="10"/>
-    </row>
-    <row r="185" spans="1:8">
-      <c r="A185" s="7"/>
-      <c r="B185" s="7"/>
-      <c r="C185" s="7"/>
-      <c r="D185" s="7"/>
-      <c r="E185" s="7"/>
-      <c r="F185" s="7"/>
-      <c r="G185" s="7"/>
-      <c r="H185" s="10"/>
-    </row>
-    <row r="186" spans="1:8">
-      <c r="A186" s="7"/>
-      <c r="B186" s="7"/>
-      <c r="C186" s="7"/>
-      <c r="D186" s="7"/>
-      <c r="E186" s="7"/>
-      <c r="F186" s="7"/>
-      <c r="G186" s="7"/>
-      <c r="H186" s="10"/>
-    </row>
-    <row r="187" spans="1:8">
-      <c r="A187" s="7"/>
-      <c r="B187" s="7"/>
-      <c r="C187" s="7"/>
-      <c r="D187" s="7"/>
-      <c r="E187" s="7"/>
-      <c r="F187" s="7"/>
-      <c r="G187" s="7"/>
-      <c r="H187" s="10"/>
-    </row>
-    <row r="188" spans="1:8">
-      <c r="A188" s="7"/>
-      <c r="B188" s="7"/>
-      <c r="C188" s="7"/>
-      <c r="D188" s="7"/>
-      <c r="E188" s="7"/>
-      <c r="F188" s="7"/>
-      <c r="G188" s="7"/>
-      <c r="H188" s="10"/>
-    </row>
-    <row r="189" spans="1:8">
-      <c r="A189" s="7"/>
-      <c r="B189" s="7"/>
-      <c r="C189" s="7"/>
-      <c r="D189" s="7"/>
-      <c r="E189" s="7"/>
-      <c r="F189" s="7"/>
-      <c r="G189" s="7"/>
+    <row r="156" spans="1:9" ht="50.25" customHeight="1">
+      <c r="A156" t="s">
+        <v>563</v>
+      </c>
+      <c r="B156" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" t="s">
+        <v>564</v>
+      </c>
+      <c r="D156" t="s">
+        <v>10</v>
+      </c>
+      <c r="E156" s="22" t="s">
+        <v>565</v>
+      </c>
+      <c r="F156" s="22" t="s">
+        <v>566</v>
+      </c>
+      <c r="G156"/>
+      <c r="I156" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" ht="57.75" customHeight="1">
+      <c r="A157" t="s">
+        <v>567</v>
+      </c>
+      <c r="B157" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" t="s">
+        <v>564</v>
+      </c>
+      <c r="D157" t="s">
+        <v>10</v>
+      </c>
+      <c r="E157" s="22" t="s">
+        <v>568</v>
+      </c>
+      <c r="F157" s="22" t="s">
+        <v>569</v>
+      </c>
+      <c r="G157"/>
+      <c r="I157" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" ht="75" customHeight="1">
+      <c r="A158" t="s">
+        <v>570</v>
+      </c>
+      <c r="B158" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" t="s">
+        <v>564</v>
+      </c>
+      <c r="D158" t="s">
+        <v>10</v>
+      </c>
+      <c r="E158" s="22" t="s">
+        <v>571</v>
+      </c>
+      <c r="F158" s="22" t="s">
+        <v>572</v>
+      </c>
+      <c r="G158"/>
+      <c r="I158" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" ht="65.25" customHeight="1">
+      <c r="A159" t="s">
+        <v>573</v>
+      </c>
+      <c r="B159" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" t="s">
+        <v>564</v>
+      </c>
+      <c r="D159" t="s">
+        <v>10</v>
+      </c>
+      <c r="E159" s="22" t="s">
+        <v>574</v>
+      </c>
+      <c r="F159" s="22" t="s">
+        <v>575</v>
+      </c>
+      <c r="G159"/>
+      <c r="I159" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" ht="66.75" customHeight="1">
+      <c r="A160" t="s">
+        <v>576</v>
+      </c>
+      <c r="B160" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" t="s">
+        <v>564</v>
+      </c>
+      <c r="D160" t="s">
+        <v>10</v>
+      </c>
+      <c r="E160" s="22" t="s">
+        <v>577</v>
+      </c>
+      <c r="F160" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="G160"/>
+      <c r="I160" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="54" customHeight="1">
+      <c r="A161" t="s">
+        <v>579</v>
+      </c>
+      <c r="B161" t="s">
+        <v>11</v>
+      </c>
+      <c r="C161" t="s">
+        <v>564</v>
+      </c>
+      <c r="D161" t="s">
+        <v>10</v>
+      </c>
+      <c r="E161" s="22" t="s">
+        <v>580</v>
+      </c>
+      <c r="F161" s="22" t="s">
+        <v>581</v>
+      </c>
+      <c r="G161"/>
+      <c r="I161" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" ht="60" customHeight="1">
+      <c r="A162" t="s">
+        <v>584</v>
+      </c>
+      <c r="B162" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" t="s">
+        <v>585</v>
+      </c>
+      <c r="D162" t="s">
+        <v>10</v>
+      </c>
+      <c r="E162" s="22" t="s">
+        <v>586</v>
+      </c>
+      <c r="F162" s="23" t="s">
+        <v>587</v>
+      </c>
+      <c r="G162"/>
+      <c r="I162" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" ht="67.5" customHeight="1">
+      <c r="A163" t="s">
+        <v>588</v>
+      </c>
+      <c r="B163" t="s">
+        <v>11</v>
+      </c>
+      <c r="C163" t="s">
+        <v>585</v>
+      </c>
+      <c r="D163" t="s">
+        <v>10</v>
+      </c>
+      <c r="E163" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="F163" s="22" t="s">
+        <v>590</v>
+      </c>
+      <c r="G163"/>
+      <c r="I163" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" ht="55.5" customHeight="1">
+      <c r="A164" t="s">
+        <v>591</v>
+      </c>
+      <c r="B164" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" t="s">
+        <v>585</v>
+      </c>
+      <c r="D164" t="s">
+        <v>10</v>
+      </c>
+      <c r="E164" s="23" t="s">
+        <v>592</v>
+      </c>
+      <c r="F164" t="s">
+        <v>593</v>
+      </c>
+      <c r="G164"/>
+      <c r="I164" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" ht="62.25" customHeight="1">
+      <c r="A165" t="s">
+        <v>594</v>
+      </c>
+      <c r="B165" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" t="s">
+        <v>585</v>
+      </c>
+      <c r="D165" t="s">
+        <v>10</v>
+      </c>
+      <c r="E165" s="22" t="s">
+        <v>595</v>
+      </c>
+      <c r="F165" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="G165"/>
+      <c r="I165" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="61.5" customHeight="1">
+      <c r="A166" t="s">
+        <v>597</v>
+      </c>
+      <c r="B166" t="s">
+        <v>11</v>
+      </c>
+      <c r="C166" t="s">
+        <v>585</v>
+      </c>
+      <c r="D166" t="s">
+        <v>10</v>
+      </c>
+      <c r="E166" s="24" t="s">
+        <v>598</v>
+      </c>
+      <c r="F166" s="22" t="s">
+        <v>599</v>
+      </c>
+      <c r="G166"/>
+      <c r="I166" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="74.25" customHeight="1">
+      <c r="A167" s="7" t="s">
+        <v>680</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C167" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D167" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E167" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="F167" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="G167" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H167" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I167" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="88.5" customHeight="1">
+      <c r="A168" s="7" t="s">
+        <v>681</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C168" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D168" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E168" s="19" t="s">
+        <v>603</v>
+      </c>
+      <c r="F168" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="G168" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H168" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I168" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="68.25" customHeight="1">
+      <c r="A169" s="7" t="s">
+        <v>682</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C169" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D169" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E169" s="19" t="s">
+        <v>604</v>
+      </c>
+      <c r="F169" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="G169" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H169" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I169" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" ht="72" customHeight="1">
+      <c r="A170" s="7" t="s">
+        <v>683</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C170" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D170" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E170" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F170" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="G170" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H170" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I170" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" ht="45">
+      <c r="A171" t="s">
+        <v>667</v>
+      </c>
+      <c r="B171" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" t="s">
+        <v>607</v>
+      </c>
+      <c r="D171" t="s">
+        <v>10</v>
+      </c>
+      <c r="E171" s="22" t="s">
+        <v>608</v>
+      </c>
+      <c r="F171" s="22" t="s">
+        <v>609</v>
+      </c>
+      <c r="G171"/>
+      <c r="I171" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" ht="90">
+      <c r="A172" t="s">
+        <v>668</v>
+      </c>
+      <c r="B172" t="s">
+        <v>11</v>
+      </c>
+      <c r="C172" t="s">
+        <v>607</v>
+      </c>
+      <c r="D172" t="s">
+        <v>10</v>
+      </c>
+      <c r="E172" s="22" t="s">
+        <v>610</v>
+      </c>
+      <c r="F172" s="22" t="s">
+        <v>611</v>
+      </c>
+      <c r="G172"/>
+      <c r="I172" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" ht="84" customHeight="1">
+      <c r="A173" t="s">
+        <v>669</v>
+      </c>
+      <c r="B173" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" t="s">
+        <v>607</v>
+      </c>
+      <c r="D173" t="s">
+        <v>10</v>
+      </c>
+      <c r="E173" s="22" t="s">
+        <v>612</v>
+      </c>
+      <c r="F173" s="22" t="s">
+        <v>613</v>
+      </c>
+      <c r="G173"/>
+      <c r="I173" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" ht="82.5" customHeight="1">
+      <c r="A174" t="s">
+        <v>670</v>
+      </c>
+      <c r="B174" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" t="s">
+        <v>607</v>
+      </c>
+      <c r="D174" t="s">
+        <v>10</v>
+      </c>
+      <c r="E174" s="22" t="s">
+        <v>614</v>
+      </c>
+      <c r="F174" s="24" t="s">
+        <v>615</v>
+      </c>
+      <c r="G174"/>
+      <c r="I174" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" ht="89.25" customHeight="1">
+      <c r="A175" t="s">
+        <v>671</v>
+      </c>
+      <c r="B175" t="s">
+        <v>11</v>
+      </c>
+      <c r="C175" t="s">
+        <v>607</v>
+      </c>
+      <c r="D175" t="s">
+        <v>10</v>
+      </c>
+      <c r="E175" s="22" t="s">
+        <v>616</v>
+      </c>
+      <c r="F175" s="24" t="s">
+        <v>617</v>
+      </c>
+      <c r="G175"/>
+      <c r="I175" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" ht="75" customHeight="1">
+      <c r="A176" t="s">
+        <v>672</v>
+      </c>
+      <c r="B176" t="s">
+        <v>11</v>
+      </c>
+      <c r="C176" t="s">
+        <v>607</v>
+      </c>
+      <c r="D176" t="s">
+        <v>10</v>
+      </c>
+      <c r="E176" s="22" t="s">
+        <v>618</v>
+      </c>
+      <c r="F176" s="24" t="s">
+        <v>619</v>
+      </c>
+      <c r="G176"/>
+      <c r="I176" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" ht="78.75" customHeight="1">
+      <c r="A177" t="s">
+        <v>621</v>
+      </c>
+      <c r="B177" t="s">
+        <v>11</v>
+      </c>
+      <c r="C177" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D177" t="s">
+        <v>10</v>
+      </c>
+      <c r="E177" s="23" t="s">
+        <v>623</v>
+      </c>
+      <c r="F177" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="G177"/>
+      <c r="I177" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" ht="105.75" customHeight="1">
+      <c r="A178" t="s">
+        <v>625</v>
+      </c>
+      <c r="B178" t="s">
+        <v>11</v>
+      </c>
+      <c r="C178" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D178" t="s">
+        <v>10</v>
+      </c>
+      <c r="E178" s="22" t="s">
+        <v>626</v>
+      </c>
+      <c r="F178" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="G178"/>
+      <c r="I178" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" ht="91.5" customHeight="1">
+      <c r="A179" t="s">
+        <v>628</v>
+      </c>
+      <c r="B179" t="s">
+        <v>11</v>
+      </c>
+      <c r="C179" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D179" t="s">
+        <v>10</v>
+      </c>
+      <c r="E179" s="22" t="s">
+        <v>629</v>
+      </c>
+      <c r="F179" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="G179"/>
+      <c r="I179" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" ht="84" customHeight="1">
+      <c r="A180" t="s">
+        <v>630</v>
+      </c>
+      <c r="B180" t="s">
+        <v>11</v>
+      </c>
+      <c r="C180" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D180" t="s">
+        <v>10</v>
+      </c>
+      <c r="E180" s="24" t="s">
+        <v>631</v>
+      </c>
+      <c r="F180" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="G180"/>
+      <c r="I180" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" ht="73.5" customHeight="1">
+      <c r="A181" t="s">
+        <v>633</v>
+      </c>
+      <c r="B181" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" s="22" t="s">
+        <v>622</v>
+      </c>
+      <c r="D181" t="s">
+        <v>10</v>
+      </c>
+      <c r="E181" s="24" t="s">
+        <v>634</v>
+      </c>
+      <c r="F181" s="24" t="s">
+        <v>632</v>
+      </c>
+      <c r="G181"/>
+      <c r="I181" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" ht="64.5" customHeight="1">
+      <c r="A182" t="s">
+        <v>673</v>
+      </c>
+      <c r="B182" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C182" t="s">
+        <v>607</v>
+      </c>
+      <c r="D182" t="s">
+        <v>10</v>
+      </c>
+      <c r="E182" s="22" t="s">
+        <v>636</v>
+      </c>
+      <c r="F182" s="22" t="s">
+        <v>637</v>
+      </c>
+      <c r="G182"/>
+      <c r="I182" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" ht="70.5" customHeight="1">
+      <c r="A183" t="s">
+        <v>674</v>
+      </c>
+      <c r="B183" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C183" t="s">
+        <v>607</v>
+      </c>
+      <c r="D183" t="s">
+        <v>10</v>
+      </c>
+      <c r="E183" s="22" t="s">
+        <v>638</v>
+      </c>
+      <c r="F183" s="22" t="s">
+        <v>639</v>
+      </c>
+      <c r="G183"/>
+      <c r="I183" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" ht="75" customHeight="1">
+      <c r="A184" t="s">
+        <v>675</v>
+      </c>
+      <c r="B184" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C184" t="s">
+        <v>607</v>
+      </c>
+      <c r="D184" t="s">
+        <v>10</v>
+      </c>
+      <c r="E184" s="22" t="s">
+        <v>640</v>
+      </c>
+      <c r="F184" s="22" t="s">
+        <v>641</v>
+      </c>
+      <c r="G184"/>
+      <c r="I184" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" ht="76.5" customHeight="1">
+      <c r="A185" t="s">
+        <v>676</v>
+      </c>
+      <c r="B185" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" t="s">
+        <v>607</v>
+      </c>
+      <c r="D185" t="s">
+        <v>10</v>
+      </c>
+      <c r="E185" s="25" t="s">
+        <v>642</v>
+      </c>
+      <c r="F185" s="22" t="s">
+        <v>643</v>
+      </c>
+      <c r="G185"/>
+      <c r="I185" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" ht="69.75" customHeight="1">
+      <c r="A186" t="s">
+        <v>677</v>
+      </c>
+      <c r="B186" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186" t="s">
+        <v>607</v>
+      </c>
+      <c r="D186" t="s">
+        <v>10</v>
+      </c>
+      <c r="E186" s="23" t="s">
+        <v>644</v>
+      </c>
+      <c r="F186" s="22" t="s">
+        <v>645</v>
+      </c>
+      <c r="G186"/>
+      <c r="I186" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" ht="80.25" customHeight="1">
+      <c r="A187" t="s">
+        <v>678</v>
+      </c>
+      <c r="B187" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C187" t="s">
+        <v>607</v>
+      </c>
+      <c r="D187" t="s">
+        <v>10</v>
+      </c>
+      <c r="E187" s="22" t="s">
+        <v>646</v>
+      </c>
+      <c r="F187" s="22" t="s">
+        <v>647</v>
+      </c>
+      <c r="G187"/>
+      <c r="I187" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" ht="89.25" customHeight="1">
+      <c r="A188" t="s">
+        <v>679</v>
+      </c>
+      <c r="B188" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C188" t="s">
+        <v>607</v>
+      </c>
+      <c r="D188" t="s">
+        <v>10</v>
+      </c>
+      <c r="E188" s="22" t="s">
+        <v>648</v>
+      </c>
+      <c r="F188" s="22" t="s">
+        <v>649</v>
+      </c>
+      <c r="G188"/>
+      <c r="I188" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" ht="45">
+      <c r="A189" s="10" t="s">
+        <v>690</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D189" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E189" s="19" t="s">
+        <v>650</v>
+      </c>
+      <c r="F189" s="19" t="s">
+        <v>651</v>
+      </c>
+      <c r="G189" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="H189" s="10"/>
-    </row>
-    <row r="190" spans="1:8">
-      <c r="A190" s="7"/>
-      <c r="B190" s="7"/>
-      <c r="C190" s="7"/>
-      <c r="D190" s="7"/>
-      <c r="E190" s="7"/>
-      <c r="F190" s="7"/>
-      <c r="G190" s="7"/>
+      <c r="I189" s="26" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" ht="45">
+      <c r="A190" s="10" t="s">
+        <v>691</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C190" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D190" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E190" s="19" t="s">
+        <v>652</v>
+      </c>
+      <c r="F190" s="19" t="s">
+        <v>653</v>
+      </c>
+      <c r="G190" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="H190" s="10"/>
-    </row>
-    <row r="191" spans="1:8">
-      <c r="A191" s="7"/>
-      <c r="B191" s="7"/>
-      <c r="C191" s="7"/>
-      <c r="D191" s="7"/>
-      <c r="E191" s="7"/>
-      <c r="F191" s="7"/>
-      <c r="G191" s="7"/>
+      <c r="I190" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" ht="45">
+      <c r="A191" s="10" t="s">
+        <v>692</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D191" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E191" s="19" t="s">
+        <v>654</v>
+      </c>
+      <c r="F191" s="19" t="s">
+        <v>655</v>
+      </c>
+      <c r="G191" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="H191" s="10"/>
-    </row>
-    <row r="192" spans="1:8">
-      <c r="A192" s="7"/>
-      <c r="B192" s="7"/>
-      <c r="C192" s="7"/>
-      <c r="D192" s="7"/>
-      <c r="E192" s="7"/>
-      <c r="F192" s="7"/>
-      <c r="G192" s="7"/>
+      <c r="I191" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" ht="72.75" customHeight="1">
+      <c r="A192" s="7" t="s">
+        <v>684</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D192" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E192" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="F192" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="G192" s="10" t="s">
+        <v>8</v>
+      </c>
       <c r="H192" s="10"/>
-    </row>
-    <row r="193" spans="1:7">
-      <c r="A193" s="7"/>
-      <c r="B193" s="7"/>
-      <c r="C193" s="7"/>
-      <c r="D193" s="7"/>
-      <c r="E193" s="7"/>
-      <c r="F193" s="7"/>
-      <c r="G193" s="7"/>
-    </row>
-    <row r="194" spans="1:7">
-      <c r="A194" s="7"/>
-      <c r="B194" s="7"/>
-      <c r="C194" s="7"/>
-      <c r="D194" s="7"/>
-      <c r="E194" s="7"/>
-      <c r="F194" s="7"/>
-      <c r="G194" s="7"/>
-    </row>
-    <row r="195" spans="1:7">
-      <c r="A195" s="7"/>
-      <c r="B195" s="7"/>
-      <c r="C195" s="7"/>
-      <c r="D195" s="7"/>
-      <c r="E195" s="7"/>
-      <c r="F195" s="7"/>
-      <c r="G195" s="7"/>
-    </row>
-    <row r="196" spans="1:7">
-      <c r="A196" s="7"/>
-      <c r="B196" s="7"/>
-      <c r="C196" s="7"/>
-      <c r="D196" s="7"/>
-      <c r="E196" s="7"/>
-      <c r="F196" s="7"/>
-      <c r="G196" s="7"/>
-    </row>
-    <row r="197" spans="1:7">
-      <c r="A197" s="7"/>
-      <c r="B197" s="7"/>
-      <c r="C197" s="7"/>
-      <c r="D197" s="7"/>
-      <c r="E197" s="7"/>
-      <c r="F197" s="7"/>
-      <c r="G197" s="7"/>
-    </row>
-    <row r="198" spans="1:7">
-      <c r="A198" s="7"/>
-      <c r="B198" s="7"/>
-      <c r="C198" s="7"/>
-      <c r="D198" s="7"/>
-      <c r="E198" s="7"/>
-      <c r="F198" s="7"/>
-      <c r="G198" s="7"/>
-    </row>
-    <row r="199" spans="1:7">
-      <c r="A199" s="7"/>
-      <c r="B199" s="7"/>
-      <c r="C199" s="7"/>
-      <c r="D199" s="7"/>
-      <c r="E199" s="7"/>
-      <c r="F199" s="7"/>
-      <c r="G199" s="7"/>
-    </row>
-    <row r="200" spans="1:7">
-      <c r="A200" s="7"/>
-      <c r="B200" s="7"/>
-      <c r="C200" s="7"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7"/>
-      <c r="F200" s="7"/>
-      <c r="G200" s="7"/>
-    </row>
-    <row r="201" spans="1:7">
-      <c r="A201" s="7"/>
-      <c r="B201" s="7"/>
-      <c r="C201" s="7"/>
-      <c r="D201" s="7"/>
-      <c r="E201" s="7"/>
-      <c r="F201" s="7"/>
-      <c r="G201" s="7"/>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="7"/>
-      <c r="B202" s="7"/>
-      <c r="C202" s="7"/>
-      <c r="D202" s="7"/>
-      <c r="E202" s="7"/>
-      <c r="F202" s="7"/>
-      <c r="G202" s="7"/>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="7"/>
-      <c r="B203" s="7"/>
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7"/>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="7"/>
-      <c r="B204" s="7"/>
-      <c r="C204" s="7"/>
-      <c r="D204" s="7"/>
-      <c r="E204" s="7"/>
-      <c r="F204" s="7"/>
-      <c r="G204" s="7"/>
-    </row>
-    <row r="205" spans="1:7">
+      <c r="I192" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="84" customHeight="1">
+      <c r="A193" s="7" t="s">
+        <v>685</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C193" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D193" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E193" s="19" t="s">
+        <v>517</v>
+      </c>
+      <c r="F193" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="G193" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H193" s="10"/>
+      <c r="I193" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="85.5" customHeight="1">
+      <c r="A194" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="B194" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C194" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D194" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E194" s="19" t="s">
+        <v>519</v>
+      </c>
+      <c r="F194" s="19" t="s">
+        <v>520</v>
+      </c>
+      <c r="G194" s="10"/>
+      <c r="H194" s="10"/>
+      <c r="I194" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="81" customHeight="1">
+      <c r="A195" s="7" t="s">
+        <v>687</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E195" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="F195" s="19" t="s">
+        <v>522</v>
+      </c>
+      <c r="G195" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H195" s="10"/>
+      <c r="I195" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="84.75" customHeight="1">
+      <c r="A196" s="7" t="s">
+        <v>688</v>
+      </c>
+      <c r="B196" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C196" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E196" s="19" t="s">
+        <v>523</v>
+      </c>
+      <c r="F196" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="G196" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H196" s="10"/>
+      <c r="I196" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="83.25" customHeight="1">
+      <c r="A197" s="10" t="s">
+        <v>658</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C197" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D197" s="10"/>
+      <c r="E197" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="F197" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="G197" s="10"/>
+      <c r="H197" s="10"/>
+      <c r="I197" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="75.75" customHeight="1">
+      <c r="A198" s="10" t="s">
+        <v>659</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C198" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D198" s="10"/>
+      <c r="E198" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="F198" s="19" t="s">
+        <v>534</v>
+      </c>
+      <c r="G198" s="10"/>
+      <c r="H198" s="10"/>
+      <c r="I198" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" ht="78.75" customHeight="1">
+      <c r="A199" s="10" t="s">
+        <v>660</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C199" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D199" s="10"/>
+      <c r="E199" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="F199" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="G199" s="10"/>
+      <c r="H199" s="10"/>
+      <c r="I199" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" ht="77.25" customHeight="1">
+      <c r="A200" s="10" t="s">
+        <v>661</v>
+      </c>
+      <c r="B200" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D200" s="10"/>
+      <c r="E200" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="F200" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="G200" s="10"/>
+      <c r="H200" s="10"/>
+      <c r="I200" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" ht="81.75" customHeight="1">
+      <c r="A201" s="10" t="s">
+        <v>662</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C201" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D201" s="10"/>
+      <c r="E201" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="F201" s="19" t="s">
+        <v>539</v>
+      </c>
+      <c r="G201" s="10"/>
+      <c r="H201" s="10"/>
+      <c r="I201" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" ht="82.5" customHeight="1">
+      <c r="A202" s="10" t="s">
+        <v>663</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C202" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D202" s="10"/>
+      <c r="E202" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="F202" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="G202" s="10"/>
+      <c r="H202" s="10"/>
+      <c r="I202" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" ht="103.5" customHeight="1">
+      <c r="A203" s="10" t="s">
+        <v>664</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D203" s="10"/>
+      <c r="E203" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="F203" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="G203" s="10"/>
+      <c r="H203" s="10"/>
+      <c r="I203" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" ht="86.25" customHeight="1">
+      <c r="A204" s="10" t="s">
+        <v>665</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C204" s="10" t="s">
+        <v>622</v>
+      </c>
+      <c r="D204" s="10"/>
+      <c r="E204" s="19" t="s">
+        <v>543</v>
+      </c>
+      <c r="F204" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="G204" s="10"/>
+      <c r="H204" s="10"/>
+      <c r="I204" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9">
       <c r="A205" s="7"/>
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
@@ -6380,7 +7531,7 @@
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:9">
       <c r="A206" s="7"/>
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
@@ -6389,7 +7540,7 @@
       <c r="F206" s="7"/>
       <c r="G206" s="7"/>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:9">
       <c r="A207" s="7"/>
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
@@ -6398,7 +7549,7 @@
       <c r="F207" s="7"/>
       <c r="G207" s="7"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:9">
       <c r="A208" s="7"/>
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
@@ -9505,16 +10656,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B138 B156:B552">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B138 B205:B552">
       <formula1>"Admin, IDA, Partner Mgmt, Pre Registration, Registration Client, Registration Processor, Resident Services"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D299">
       <formula1>"Acceptance, Functional, Smoke, Security, Performance"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H139:H154 G2:G299">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H139:H154 G2:G155 G205:G299 G156:H204">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B139:B155">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B139:B204">
       <formula1>"Admin, Credential Services, IDA, Partner Mgmt, Pre Registration, Registration Client, Registration Processor, Resident Services"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9527,7 +10678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -9566,7 +10717,7 @@
     </row>
     <row r="2" spans="1:7" ht="39" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
@@ -9576,10 +10727,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>8</v>
@@ -9587,20 +10738,20 @@
     </row>
     <row r="3" spans="1:7" ht="39" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>8</v>
@@ -9608,20 +10759,20 @@
     </row>
     <row r="4" spans="1:7" ht="39" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>8</v>
@@ -9629,20 +10780,20 @@
     </row>
     <row r="5" spans="1:7" ht="39" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>412</v>
-      </c>
       <c r="F5" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>8</v>
@@ -9650,20 +10801,20 @@
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1">
       <c r="A6" s="10" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>8</v>
@@ -9671,20 +10822,20 @@
     </row>
     <row r="7" spans="1:7" ht="39" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>7</v>
@@ -9692,20 +10843,20 @@
     </row>
     <row r="8" spans="1:7" ht="39" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>417</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>421</v>
-      </c>
       <c r="F8" s="11" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>7</v>
@@ -9713,20 +10864,20 @@
     </row>
     <row r="9" spans="1:7" ht="39" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>7</v>
@@ -9734,20 +10885,20 @@
     </row>
     <row r="10" spans="1:7" ht="39" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>7</v>
@@ -9755,20 +10906,20 @@
     </row>
     <row r="11" spans="1:7" ht="39" customHeight="1">
       <c r="A11" s="10" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>8</v>
@@ -9776,20 +10927,20 @@
     </row>
     <row r="12" spans="1:7" ht="39" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>8</v>
@@ -9797,20 +10948,20 @@
     </row>
     <row r="13" spans="1:7" ht="39" customHeight="1">
       <c r="A13" s="10" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>8</v>
@@ -9818,20 +10969,20 @@
     </row>
     <row r="14" spans="1:7" ht="39" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>7</v>
@@ -9839,20 +10990,20 @@
     </row>
     <row r="15" spans="1:7" ht="39" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>8</v>
@@ -9860,20 +11011,20 @@
     </row>
     <row r="16" spans="1:7" ht="39" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>7</v>
@@ -9881,20 +11032,20 @@
     </row>
     <row r="17" spans="1:7" ht="39" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>8</v>
@@ -9902,20 +11053,20 @@
     </row>
     <row r="18" spans="1:7" ht="39" customHeight="1">
       <c r="A18" s="10" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="10" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>8</v>
@@ -9944,7 +11095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9990,10 +11141,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>8</v>
@@ -10001,22 +11152,22 @@
     </row>
     <row r="3" spans="1:7" ht="25.5">
       <c r="A3" s="14" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>8</v>
@@ -10024,22 +11175,22 @@
     </row>
     <row r="4" spans="1:7" ht="38.25">
       <c r="A4" s="14" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>461</v>
-      </c>
       <c r="F4" s="15" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>8</v>
@@ -10047,22 +11198,22 @@
     </row>
     <row r="5" spans="1:7" ht="38.25">
       <c r="A5" s="14" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>8</v>
@@ -10082,10 +11233,10 @@
         <v>10</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>8</v>
@@ -10105,10 +11256,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G7" s="16" t="s">
         <v>8</v>
@@ -10128,10 +11279,10 @@
         <v>10</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>8</v>
@@ -10151,10 +11302,10 @@
         <v>10</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G9" s="16" t="s">
         <v>8</v>
@@ -10174,10 +11325,10 @@
         <v>10</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>8</v>
@@ -10197,10 +11348,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G11" s="16" t="s">
         <v>8</v>
@@ -10220,10 +11371,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>8</v>
@@ -10243,10 +11394,10 @@
         <v>10</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>8</v>
@@ -10266,10 +11417,10 @@
         <v>10</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>8</v>
@@ -10277,7 +11428,7 @@
     </row>
     <row r="15" spans="1:7" ht="25.5">
       <c r="A15" s="14" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>11</v>
@@ -10289,10 +11440,10 @@
         <v>10</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>8</v>
@@ -10300,7 +11451,7 @@
     </row>
     <row r="16" spans="1:7" ht="25.5">
       <c r="A16" s="14" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>11</v>
@@ -10312,10 +11463,10 @@
         <v>10</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>8</v>
@@ -10323,22 +11474,22 @@
     </row>
     <row r="17" spans="1:7" ht="89.25">
       <c r="A17" s="14" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>8</v>
@@ -10346,22 +11497,22 @@
     </row>
     <row r="18" spans="1:7" ht="38.25">
       <c r="A18" s="14" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>8</v>
@@ -10369,22 +11520,22 @@
     </row>
     <row r="19" spans="1:7" ht="38.25">
       <c r="A19" s="14" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="G19" s="16" t="s">
         <v>8</v>
@@ -10392,22 +11543,22 @@
     </row>
     <row r="20" spans="1:7" ht="51">
       <c r="A20" s="14" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>8</v>
@@ -10415,19 +11566,19 @@
     </row>
     <row r="21" spans="1:7" ht="38.25">
       <c r="A21" s="14" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="10"/>
@@ -10438,125 +11589,125 @@
         <v>11</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F22" s="15"/>
       <c r="G22" s="10"/>
     </row>
     <row r="23" spans="1:7" ht="51">
       <c r="A23" s="14" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="G23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="76.5">
       <c r="A24" s="14" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>392</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="D24" s="16" t="s">
-        <v>396</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>507</v>
-      </c>
       <c r="F24" s="15" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G24" s="10"/>
     </row>
     <row r="25" spans="1:7" ht="76.5">
       <c r="A25" s="14" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="G25" s="10"/>
     </row>
     <row r="26" spans="1:7" ht="102">
       <c r="A26" s="14" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G26" s="10"/>
     </row>
     <row r="27" spans="1:7" ht="76.5">
       <c r="A27" s="14" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D27" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:7" ht="63.75">
       <c r="A28" s="10" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>11</v>
@@ -10568,10 +11719,10 @@
         <v>10</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="G28" s="10"/>
     </row>

</xml_diff>